<commit_message>
the role issues and the design of the problems in xls sheet solved
</commit_message>
<xml_diff>
--- a/bugs_track_assign.xlsx
+++ b/bugs_track_assign.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ci_system_setup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="15300" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15300" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Bugs</t>
     <phoneticPr fontId="1"/>
@@ -30,41 +35,59 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t xml:space="preserve">After role is added then choose role is not in the label for the next </t>
+  </si>
+  <si>
+    <t>time bit not refreshing the browser</t>
+  </si>
+  <si>
+    <t>In create role there is Sign Up button, Make it Add</t>
+  </si>
+  <si>
+    <t>Error in adding user: there is problem in user adding</t>
+  </si>
+  <si>
+    <t>Rupesh</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rupesh</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9-4-014</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>While role is added then it will added for two times</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After role is added then choose role is not in the label for the next </t>
-  </si>
-  <si>
-    <t>time bit not refreshing the browser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>solved</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Label is Choose Group instead of Choose Role for dropdown</t>
-  </si>
-  <si>
-    <t>In create role there is Sign Up button, Make it Add</t>
-  </si>
-  <si>
-    <t>Error in adding user: there is problem in user adding</t>
-  </si>
-  <si>
-    <t>Rupesh</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Rupesh</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>9-4-014</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on creating new roles we have to choose group so I think choose group is ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>confused ??</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">solved </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>solved</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -135,6 +158,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -182,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,18 +455,18 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.8">
+    <row r="1" spans="1:4" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,82 +477,87 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -555,7 +586,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>